<commit_message>
Fixed CO2 flow labels
</commit_message>
<xml_diff>
--- a/rmnd_lca/data/additional_inventories/lci-hydrogen-smr-biogas.xlsx
+++ b/rmnd_lca/data/additional_inventories/lci-hydrogen-smr-biogas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -507,7 +507,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -559,13 +559,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="7" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -593,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -615,9 +608,8 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -903,16 +895,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="B189" sqref="B189"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.88671875" customWidth="1"/>
+    <col min="1" max="1" width="64.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -920,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -928,7 +920,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -936,7 +928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -944,7 +936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -952,7 +944,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -960,7 +952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -968,12 +960,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1014,7 +1006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -1043,7 +1035,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>146</v>
       </c>
@@ -1081,7 +1073,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>149</v>
       </c>
@@ -1119,11 +1111,11 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="15">
         <f>6.32/120</f>
         <v>5.2666666666666667E-2</v>
       </c>
@@ -1158,7 +1150,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>153</v>
       </c>
@@ -1196,7 +1188,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -1204,7 +1196,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1212,7 +1204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1220,7 +1212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1228,7 +1220,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1236,7 +1228,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1244,12 +1236,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1290,7 +1282,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>154</v>
       </c>
@@ -1319,7 +1311,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>146</v>
       </c>
@@ -1357,7 +1349,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>149</v>
       </c>
@@ -1395,11 +1387,11 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="16">
+      <c r="B28" s="15">
         <f>6.32/120</f>
         <v>5.2666666666666667E-2</v>
       </c>
@@ -1434,7 +1426,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>156</v>
       </c>
@@ -1472,7 +1464,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
@@ -1480,7 +1472,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1488,7 +1480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1496,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1504,7 +1496,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1512,7 +1504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -1520,12 +1512,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -1566,7 +1558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>157</v>
       </c>
@@ -1595,7 +1587,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>146</v>
       </c>
@@ -1633,7 +1625,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>149</v>
       </c>
@@ -1671,11 +1663,11 @@
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B42" s="16">
+      <c r="B42" s="15">
         <f>6.32/120</f>
         <v>5.2666666666666667E-2</v>
       </c>
@@ -1710,7 +1702,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>156</v>
       </c>
@@ -1748,7 +1740,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
@@ -1756,7 +1748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -1764,7 +1756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1772,7 +1764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -1780,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1788,7 +1780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -1796,7 +1788,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -1804,7 +1796,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -1812,12 +1804,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -1840,7 +1832,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>3</v>
       </c>
@@ -1863,7 +1855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>22</v>
       </c>
@@ -1886,7 +1878,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>27</v>
       </c>
@@ -1909,7 +1901,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>31</v>
       </c>
@@ -1932,7 +1924,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>32</v>
       </c>
@@ -1955,7 +1947,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -1978,7 +1970,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
@@ -1986,7 +1978,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>4</v>
       </c>
@@ -1994,7 +1986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -2002,7 +1994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -2010,7 +2002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>9</v>
       </c>
@@ -2018,7 +2010,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -2026,7 +2018,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -2034,7 +2026,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -2042,12 +2034,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>17</v>
       </c>
@@ -2070,7 +2062,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>35</v>
       </c>
@@ -2093,7 +2085,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>36</v>
       </c>
@@ -2116,7 +2108,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>27</v>
       </c>
@@ -2139,7 +2131,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>31</v>
       </c>
@@ -2162,7 +2154,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>32</v>
       </c>
@@ -2185,7 +2177,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>34</v>
       </c>
@@ -2208,7 +2200,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>2</v>
       </c>
@@ -2216,7 +2208,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>37</v>
       </c>
@@ -2224,7 +2216,7 @@
         <v>1.283708329984486</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>4</v>
       </c>
@@ -2232,7 +2224,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -2240,7 +2232,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>9</v>
       </c>
@@ -2248,7 +2240,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -2256,12 +2248,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>17</v>
       </c>
@@ -2287,7 +2279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>36</v>
       </c>
@@ -2310,7 +2302,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>40</v>
       </c>
@@ -2336,7 +2328,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>45</v>
       </c>
@@ -2362,7 +2354,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>46</v>
       </c>
@@ -2388,7 +2380,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>47</v>
       </c>
@@ -2414,7 +2406,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -2440,7 +2432,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>49</v>
       </c>
@@ -2466,7 +2458,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>50</v>
       </c>
@@ -2492,7 +2484,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>51</v>
       </c>
@@ -2518,7 +2510,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>52</v>
       </c>
@@ -2544,7 +2536,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>53</v>
       </c>
@@ -2570,7 +2562,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>54</v>
       </c>
@@ -2596,7 +2588,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>55</v>
       </c>
@@ -2622,7 +2614,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>56</v>
       </c>
@@ -2648,7 +2640,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>57</v>
       </c>
@@ -2674,7 +2666,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>58</v>
       </c>
@@ -2700,7 +2692,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>59</v>
       </c>
@@ -2726,7 +2718,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>60</v>
       </c>
@@ -2752,7 +2744,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>61</v>
       </c>
@@ -2778,7 +2770,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>62</v>
       </c>
@@ -2804,7 +2796,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>63</v>
       </c>
@@ -2830,7 +2822,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>66</v>
       </c>
@@ -2853,7 +2845,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>68</v>
       </c>
@@ -2876,7 +2868,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>70</v>
       </c>
@@ -2899,7 +2891,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>73</v>
       </c>
@@ -2922,7 +2914,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>76</v>
       </c>
@@ -2945,7 +2937,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>78</v>
       </c>
@@ -2968,7 +2960,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>80</v>
       </c>
@@ -2991,7 +2983,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>82</v>
       </c>
@@ -3014,7 +3006,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>84</v>
       </c>
@@ -3037,7 +3029,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>86</v>
       </c>
@@ -3060,7 +3052,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>88</v>
       </c>
@@ -3083,7 +3075,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>90</v>
       </c>
@@ -3106,7 +3098,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>92</v>
       </c>
@@ -3129,7 +3121,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>94</v>
       </c>
@@ -3152,7 +3144,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>96</v>
       </c>
@@ -3175,7 +3167,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>99</v>
       </c>
@@ -3198,7 +3190,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>101</v>
       </c>
@@ -3221,7 +3213,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>103</v>
       </c>
@@ -3245,7 +3237,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>2</v>
       </c>
@@ -3253,7 +3245,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>37</v>
       </c>
@@ -3261,7 +3253,7 @@
         <v>1.3097345915810461</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>4</v>
       </c>
@@ -3269,7 +3261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>9</v>
       </c>
@@ -3277,7 +3269,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>14</v>
       </c>
@@ -3285,7 +3277,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>12</v>
       </c>
@@ -3293,12 +3285,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>17</v>
       </c>
@@ -3324,7 +3316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>22</v>
       </c>
@@ -3347,7 +3339,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>40</v>
       </c>
@@ -3373,7 +3365,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>45</v>
       </c>
@@ -3399,7 +3391,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>46</v>
       </c>
@@ -3425,7 +3417,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>47</v>
       </c>
@@ -3451,7 +3443,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>48</v>
       </c>
@@ -3477,7 +3469,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>49</v>
       </c>
@@ -3503,7 +3495,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>50</v>
       </c>
@@ -3529,7 +3521,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>51</v>
       </c>
@@ -3555,7 +3547,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>52</v>
       </c>
@@ -3581,7 +3573,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>53</v>
       </c>
@@ -3607,7 +3599,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>54</v>
       </c>
@@ -3633,7 +3625,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>55</v>
       </c>
@@ -3659,7 +3651,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>56</v>
       </c>
@@ -3685,7 +3677,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>57</v>
       </c>
@@ -3711,7 +3703,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>58</v>
       </c>
@@ -3737,7 +3729,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>59</v>
       </c>
@@ -3763,7 +3755,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>60</v>
       </c>
@@ -3789,7 +3781,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>61</v>
       </c>
@@ -3815,7 +3807,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>62</v>
       </c>
@@ -3841,7 +3833,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>63</v>
       </c>
@@ -3867,7 +3859,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>68</v>
       </c>
@@ -3890,7 +3882,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>70</v>
       </c>
@@ -3913,7 +3905,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>73</v>
       </c>
@@ -3936,7 +3928,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>76</v>
       </c>
@@ -3959,7 +3951,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>78</v>
       </c>
@@ -3982,7 +3974,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>82</v>
       </c>
@@ -4005,7 +3997,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>84</v>
       </c>
@@ -4028,7 +4020,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>86</v>
       </c>
@@ -4051,7 +4043,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>88</v>
       </c>
@@ -4074,7 +4066,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>90</v>
       </c>
@@ -4097,7 +4089,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>92</v>
       </c>
@@ -4120,7 +4112,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>94</v>
       </c>
@@ -4143,7 +4135,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>96</v>
       </c>
@@ -4166,7 +4158,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>99</v>
       </c>
@@ -4189,7 +4181,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>101</v>
       </c>
@@ -4212,7 +4204,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>103</v>
       </c>
@@ -4236,7 +4228,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>2</v>
       </c>
@@ -4245,7 +4237,7 @@
       </c>
       <c r="C174" s="5"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>14</v>
       </c>
@@ -4254,7 +4246,7 @@
       </c>
       <c r="C175" s="5"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>9</v>
       </c>
@@ -4263,7 +4255,7 @@
       </c>
       <c r="C176" s="5"/>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>4</v>
       </c>
@@ -4272,7 +4264,7 @@
       </c>
       <c r="C177" s="5"/>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>8</v>
       </c>
@@ -4281,7 +4273,7 @@
       </c>
       <c r="C178" s="5"/>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>12</v>
       </c>
@@ -4290,14 +4282,14 @@
       </c>
       <c r="C179" s="5"/>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C180" s="5"/>
       <c r="D180" s="7"/>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>17</v>
       </c>
@@ -4326,7 +4318,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>68</v>
       </c>
@@ -4352,7 +4344,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" s="11" t="s">
         <v>108</v>
       </c>
@@ -4378,30 +4370,30 @@
         <v>110</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A184" s="12" t="s">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A184" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B184" s="12" t="s">
+      <c r="B184" s="11" t="s">
         <v>72</v>
       </c>
       <c r="C184" s="5">
         <v>4.0000000000000001E-10</v>
       </c>
-      <c r="D184" s="12" t="s">
+      <c r="D184" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E184" s="12" t="s">
+      <c r="E184" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="F184" s="12"/>
-      <c r="G184" s="12" t="s">
+      <c r="F184" s="11"/>
+      <c r="G184" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H184" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I184" s="12" t="s">
+      <c r="H184" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I184" s="11" t="s">
         <v>112</v>
       </c>
       <c r="J184" s="7"/>
@@ -4409,11 +4401,11 @@
       <c r="L184" s="7"/>
       <c r="M184" s="7"/>
     </row>
-    <row r="185" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A185" s="12" t="s">
+    <row r="185" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A185" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B185" s="12" t="s">
+      <c r="B185" s="11" t="s">
         <v>114</v>
       </c>
       <c r="C185" s="5">
@@ -4428,21 +4420,21 @@
       <c r="G185" t="s">
         <v>33</v>
       </c>
-      <c r="H185" s="12" t="s">
+      <c r="H185" s="11" t="s">
         <v>25</v>
       </c>
       <c r="I185" t="s">
         <v>115</v>
       </c>
-      <c r="J185" s="13"/>
-      <c r="K185" s="13"/>
-      <c r="L185" s="13"/>
-    </row>
-    <row r="186" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A186" s="12" t="s">
+      <c r="J185" s="12"/>
+      <c r="K185" s="12"/>
+      <c r="L185" s="12"/>
+    </row>
+    <row r="186" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A186" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B186" s="12" t="s">
+      <c r="B186" s="11" t="s">
         <v>98</v>
       </c>
       <c r="C186" s="5">
@@ -4457,52 +4449,52 @@
       <c r="G186" t="s">
         <v>23</v>
       </c>
-      <c r="H186" s="12" t="s">
+      <c r="H186" s="11" t="s">
         <v>25</v>
       </c>
       <c r="I186" t="s">
         <v>98</v>
       </c>
-      <c r="J186" s="13"/>
-      <c r="K186" s="13"/>
-      <c r="L186" s="13"/>
-    </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A187" s="12" t="s">
+      <c r="J186" s="12"/>
+      <c r="K186" s="12"/>
+      <c r="L186" s="12"/>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A187" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B187" s="12" t="s">
+      <c r="B187" s="11" t="s">
         <v>117</v>
       </c>
       <c r="C187" s="5">
         <v>5.4696132596685076E-5</v>
       </c>
-      <c r="D187" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E187" s="12" t="s">
+      <c r="D187" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E187" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="F187" s="12"/>
-      <c r="G187" s="12" t="s">
+      <c r="F187" s="11"/>
+      <c r="G187" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H187" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I187" s="12" t="s">
+      <c r="H187" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I187" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="J187" s="12"/>
-      <c r="K187" s="12"/>
-      <c r="L187" s="12"/>
-      <c r="M187" s="12"/>
-    </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A188" s="12" t="s">
+      <c r="J187" s="11"/>
+      <c r="K187" s="11"/>
+      <c r="L187" s="11"/>
+      <c r="M187" s="11"/>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A188" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B188" s="12" t="s">
+      <c r="B188" s="11" t="s">
         <v>120</v>
       </c>
       <c r="C188" s="5">
@@ -4524,8 +4516,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="189" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A189" s="12" t="s">
+    <row r="189" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A189" s="11" t="s">
         <v>122</v>
       </c>
       <c r="B189" t="s">
@@ -4549,12 +4541,12 @@
       <c r="I189" t="s">
         <v>124</v>
       </c>
-      <c r="J189" s="13"/>
-      <c r="K189" s="13"/>
-      <c r="L189" s="13"/>
-    </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A190" s="12" t="s">
+      <c r="J189" s="12"/>
+      <c r="K189" s="12"/>
+      <c r="L189" s="12"/>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A190" s="11" t="s">
         <v>125</v>
       </c>
       <c r="B190" t="s">
@@ -4579,8 +4571,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A191" s="14" t="s">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A191" s="13" t="s">
         <v>128</v>
       </c>
       <c r="C191" s="5">
@@ -4602,8 +4594,8 @@
         <v>129</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A192" s="14" t="s">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A192" s="13" t="s">
         <v>49</v>
       </c>
       <c r="C192" s="5">
@@ -4625,8 +4617,8 @@
         <v>130</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A193" s="14" t="s">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A193" s="13" t="s">
         <v>131</v>
       </c>
       <c r="C193" s="5">
@@ -4648,11 +4640,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A194" s="14" t="s">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A194" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B194" s="12"/>
+      <c r="B194" s="11"/>
       <c r="C194" s="5">
         <v>5.5157999999999997E-4</v>
       </c>
@@ -4672,8 +4664,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A195" s="14" t="s">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A195" s="13" t="s">
         <v>134</v>
       </c>
       <c r="C195" s="5">
@@ -4695,8 +4687,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="14" t="s">
+    <row r="196" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="13" t="s">
         <v>135</v>
       </c>
       <c r="C196" s="5">
@@ -4718,7 +4710,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>2</v>
       </c>
@@ -4726,20 +4718,20 @@
         <v>108</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A199" s="15" t="s">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B199" s="15" t="s">
+      <c r="B199" s="14" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>4</v>
       </c>
@@ -4747,7 +4739,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>8</v>
       </c>
@@ -4755,7 +4747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>12</v>
       </c>
@@ -4763,12 +4755,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>17</v>
       </c>
@@ -4797,7 +4789,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>108</v>
       </c>
@@ -4823,7 +4815,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>137</v>
       </c>
@@ -4846,7 +4838,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>49</v>
       </c>
@@ -4868,5 +4860,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>